<commit_message>
Trend graph and small changes
Finished the trend graph and changed the Game and Player class and some
small changes to fix the integration between the classes.
</commit_message>
<xml_diff>
--- a/files/test.xlsx
+++ b/files/test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Home team</t>
   </si>
@@ -19,12 +19,12 @@
     <t>Away team</t>
   </si>
   <si>
+    <t>Varberg</t>
+  </si>
+  <si>
     <t>Kungsbacka</t>
   </si>
   <si>
-    <t>Trollhättan</t>
-  </si>
-  <si>
     <t>Namn</t>
   </si>
   <si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>John Sundemo</t>
+  </si>
+  <si>
+    <t>Marten Gullberg</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -316,6 +319,56 @@
       </c>
       <c r="P5" s="1">
         <v>14.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>